<commit_message>
Update teste envio de email
</commit_message>
<xml_diff>
--- a/Ofertas.xlsx
+++ b/Ofertas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C69"/>
+  <dimension ref="A1:C51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,37 +461,37 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://www.carrefour.com.br/vitrine-iphone-12-apple-64gb-azul-tela-61-camera-traseira-dupla-12mp-mp911874363/p&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjj1fvO2Of8AhU0q5UCHckxBVEQguUECPoM&amp;usg=AOvVaw2Z3qDrYb8zy9aj37oFBN0o</t>
+          <t>https://www.google.com.br/url?url=https://www.carrefour.com.br/vitrine-iphone-12-apple-64gb-azul-tela-61-camera-traseira-dupla-12mp-mp911874363/p&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjpuMvd3uf8AhVOrZUCHSO4D-UQguUECKkL&amp;usg=AOvVaw0nbI-wTaX6_z0OQyFgTH6B</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>apple iphone 12, 64gb - branco</t>
+          <t>iphone 12 64gb</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>4274.05</v>
+        <v>3800</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://www.amazon.com.br/Apple-iPhone-12-64-GB-Branco/dp/B09B7X1814%3Fsource%3Dps-sl-shoppingads-lpcontext%26ref_%3Dfplfs%26psc%3D1%26smid%3DA1ZZFT5FULY4LN&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjj1fvO2Of8AhU0q5UCHckxBVEQguUECIsN&amp;usg=AOvVaw32rZiYENus6LE4iy88zuXe</t>
+          <t>https://www.google.com.br/url?url=https://sp.olx.com.br/regiao-de-sao-jose-do-rio-preto/celulares/iphone-12-64gb-1060086917&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjpuMvd3uf8AhVOrZUCHSO4D-UQgOUECLgL&amp;usg=AOvVaw05TErI_li_UBbgNG1GAYaC</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>iphone 12 64gb</t>
+          <t>iphone 12 64gb - azul - estou zerado</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>3800</v>
+        <v>3329.1</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://sp.olx.com.br/regiao-de-sao-jose-do-rio-preto/celulares/iphone-12-64gb-1060086917&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjj1fvO2Of8AhU0q5UCHckxBVEQgOUECJoN&amp;usg=AOvVaw1fuJAoltm3EnmGJVX9utZB</t>
+          <t>https://www.google.com.br/url?url=https://www.trocafy.com.br/iphone-12-64gb-azul-sou-como-novo-2552/p%3Fidsku%3D966%26srsltid%3DAd5pg_HlwMaBZCfGupW8GV9D-1JYAPPlCP4PeGOyMoMCtpko-10tM9yo484&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjpuMvd3uf8AhVOrZUCHSO4D-UQguUECNkL&amp;usg=AOvVaw39aVmCoKLWy3RuEFsnkKwL</t>
         </is>
       </c>
     </row>
@@ -502,221 +502,221 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>4064.09</v>
+        <v>4123</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://www.buscape.com.br/lead%3Foid%3D942845168%26sortorder%3D-1%26index%3D%26searchterm%3Dnull%26pagesize%3D-1%26channel%3D%26og%3D19221%26pla%3D2023-01-27T06:13:13.209503&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjj1fvO2Of8AhU0q5UCHckxBVEQgOUECKoN&amp;usg=AOvVaw0w9pqa3KbYcNxpuYnL4vnR</t>
+          <t>https://www.google.com.br/url?url=https://www.buscape.com.br/lead%3Foid%3D942845168%26sortorder%3D-1%26index%3D%26searchterm%3Dnull%26pagesize%3D-1%26channel%3D%26og%3D19221%26pla%3D2023-01-27T07:51:41.232289&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjpuMvd3uf8AhVOrZUCHSO4D-UQgOUECOkL&amp;usg=AOvVaw2ivQKW8tMedMhcfoo_Sm5y</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>iphone 12 64gb - azul - estou zerado</t>
+          <t>(pronta entrega) iphone 12 64gb preto</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>3329.1</v>
+        <v>4089.9</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://www.trocafy.com.br/iphone-12-64gb-azul-sou-como-novo-2552/p%3Fidsku%3D966%26srsltid%3DAd5pg_FT7bZdMI652YcsCQKTe44ObKh3cR_tbaYWruDSOAd0G54kI6FEfec&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjj1fvO2Of8AhU0q5UCHckxBVEQguUECLoN&amp;usg=AOvVaw1aC-nNp7RjwMzHDpfp8U9u</t>
+          <t>https://www.google.com.br/url?url=https://www.vtrimports.com/pronta-entrega-iphone-12-64gb-preto&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjpuMvd3uf8AhVOrZUCHSO4D-UQgOUECPgL&amp;usg=AOvVaw2z_EN-E32mS2ARKa6aqGnR</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>(pronta entrega) iphone 12 64gb preto</t>
+          <t>iphone 12 64gb tela 6.1 sem carregador e fone apple, preto</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>4089.9</v>
+        <v>4436.24</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://www.vtrimports.com/pronta-entrega-iphone-12-64gb-preto&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjj1fvO2Of8AhU0q5UCHckxBVEQgOUECMoN&amp;usg=AOvVaw362iDcTP43Zg7Sv3OJfpY4</t>
+          <t>https://www.google.com.br/url?url=https://www.magazineluiza.com.br/iphone-12-64gb-tela-6-1-sem-carregador-e-fone-apple/p/cekdf2k7k9/te/ip12/%3F%26seller_id%3Dlojasmm&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjpuMvd3uf8AhVOrZUCHSO4D-UQgOUECIcM&amp;usg=AOvVaw3GMFOj24NtFKX6nnl4IrL_</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>iphone 12 64gb tela 6.1 sem carregador e fone apple, preto</t>
+          <t>iphone 12 64gb branco seminovo</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>4436.24</v>
+        <v>2600</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://www.magazineluiza.com.br/iphone-12-64gb-tela-6-1-sem-carregador-e-fone-apple/p/cekdf2k7k9/te/ip12/%3F%26seller_id%3Dlojasmm&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjj1fvO2Of8AhU0q5UCHckxBVEQgOUECI4O&amp;usg=AOvVaw3mlxLnMtdhCRVfSS4AF1I7</t>
+          <t>https://www.google.com.br/url?url=http://loja.switchphone.com.br/iphone-12-64gb-branco-seminovo%3Fsrsltid%3DAd5pg_F0Svx9jdvg-NL403DZTiXsn0LAzneKm7F288B6GXnGsJDUWk6KYcw&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjpuMvd3uf8AhVOrZUCHSO4D-UQgOUECKUM&amp;usg=AOvVaw00zL9-Pb7wD7fczauRvAc4</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>iphone 12 64gb branco seminovo</t>
+          <t>iphone 12 64gb preto + brinde</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>2600</v>
+        <v>4249</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=http://loja.switchphone.com.br/iphone-12-64gb-branco-seminovo%3Fsrsltid%3DAd5pg_H4W-eu_TJauBtwHohA7eBlo6twEkNQ1MxDQyujKiqTWYZBoKzh9NU&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjj1fvO2Of8AhU0q5UCHckxBVEQgOUECK0O&amp;usg=AOvVaw1UbeI38_ZsLsgYG7214Nsy</t>
+          <t>https://www.google.com.br/url?url=https://www.malibushop.com.br/apple/iphone-12-64gb-preto-brinde%3Fparceiro%3D1538%26srsltid%3DAd5pg_GhB8JJ8mNDpplN7C0WEI5Ylca-tPHXjtQ9MGQgFks_5l3uBqihJvI&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjpuMvd3uf8AhVOrZUCHSO4D-UQgOUECLUM&amp;usg=AOvVaw3dDTh5LVcxDtsRbA4pg-eB</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>iphone 12 64gb - preto - estou zerado</t>
+          <t>iphone 12 preto 64gb vitrine | celular apple | usado</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>3329.1</v>
+        <v>4173</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://www.trocafy.com.br/iphone-12-64gb-preto-sou-como-novo-2551/p%3Fidsku%3D971%26srsltid%3DAd5pg_HCUTrLxqzw1eYhiuG12xHBTLQivsrvPKwdai0XNl9NEqjQZ_O8T7A&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjj1fvO2Of8AhU0q5UCHckxBVEQguUECL4O&amp;usg=AOvVaw3hhDS93QVqsJR7LjysZumU</t>
+          <t>https://www.google.com.br/url?url=https://www.enjoei.com.br/p/iphone-12-preto-64gb-vitrine-72712010%3Fg_campaign%3Dgoogle_shopping&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjpuMvd3uf8AhVOrZUCHSO4D-UQgOUECNQM&amp;usg=AOvVaw3BuFKX9lpPJlkiVdNPlE73</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>iphone 12 64gb preto + brinde</t>
+          <t>iphone 12 apple 64gb - verde tela 6,1" 12mp ios - - verde</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>4249</v>
+        <v>4499</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://www.malibushop.com.br/apple/iphone-12-64gb-preto-brinde%3Fparceiro%3D1538%26srsltid%3DAd5pg_FsG6mgoJYWI6MMNJ1Vbp5p3UcgjdsJ4Cwh5Frd4efB_iYLLJ0bzUU&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjj1fvO2Of8AhU0q5UCHckxBVEQgOUECIEP&amp;usg=AOvVaw1ABDaz9GDyDN_eG2RmoSkf</t>
+          <t>https://www.google.com.br/url?url=https://www.shoppingsmiles.com.br/smiles/produto.jsf%3Fs%3D2311477-00%26p%3D2311477_8%26a%3Dtrue&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjpuMvd3uf8AhVOrZUCHSO4D-UQgOUECOIN&amp;usg=AOvVaw1IHKsJ2tM2bsVY5qKirvvo</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>iphone 12 preto 64gb vitrine | celular apple | usado</t>
+          <t>(seminovos) iphone 12 apple preto, 64gb</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>4173</v>
+        <v>3519.12</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://www.enjoei.com.br/p/iphone-12-preto-64gb-vitrine-72712010%3Fg_campaign%3Dgoogle_shopping&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjj1fvO2Of8AhU0q5UCHckxBVEQgOUECOQP&amp;usg=AOvVaw2L9JKeAxtqVBsFMTmtq0ck</t>
+          <t>https://www.google.com.br/url?url=https://www.taqi.com.br/seminovos-usado-apple-iphone-12-preto-nacional/221635%3Fsrsltid%3DAd5pg_FzPUQ9hjAXcGNteiRTL94AZ9t-OdM_ZncaqdHJCG0MRH24UuzUXFA&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjpuMvd3uf8AhVOrZUCHSO4D-UQgOUECPEN&amp;usg=AOvVaw3kJCd7QV5xH_KfvAVnjg7n</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>iphone 12 64gb azul seminovo</t>
+          <t>iphone 12 apple 64gb - roxo tela 6,1" 12mp ios - - roxo</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>2600</v>
+        <v>4499</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=http://loja.switchphone.com.br/iphone-12-64gb-azul-seminovo%3Fsrsltid%3DAd5pg_GxL0GhmygNvmh3N4OjNwKScBr6j6vHtd__7hZrk0cff0X6b8SXWtw&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjj1fvO2Of8AhU0q5UCHckxBVEQgOUECPQP&amp;usg=AOvVaw05elsOJGgHGnTuj0C5uLOf</t>
+          <t>https://www.google.com.br/url?url=https://www.shoppingsmiles.com.br/smiles/produto.jsf%3Fs%3D2311488-00%26p%3D2311488_8%26a%3Dtrue&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjpuMvd3uf8AhVOrZUCHSO4D-UQgOUECIAO&amp;usg=AOvVaw1KaFM9TuEeaXVrkd4A6DgB</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>iphone 12 64gb lilás + brinde</t>
+          <t>(seminovo) iphone 12 apple azul, 64gb</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>4249</v>
+        <v>3399.15</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://www.malibushop.com.br/apple/iphone-12-64gb-lilas-brinde%3Fparceiro%3D1538%26srsltid%3DAd5pg_Gu3RQ34odr2jK3yMxHjDohgt-fIfKnFUGHBa6WnF15skm5ryVYRpo&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjj1fvO2Of8AhU0q5UCHckxBVEQgOUECIQQ&amp;usg=AOvVaw3fdT4KnWXAC3-KMokWdcmq</t>
+          <t>https://www.google.com.br/url?url=https://www.taqi.com.br/seminovo-apple-iphone-12-64gb-azul-internacional-taqi/222835%3Fsrsltid%3DAd5pg_G9B-kHp_h4H4iZKaMzebeyX0soGfvi7z9ZfgYHruvB7BJk1OVw0s0&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjpuMvd3uf8AhVOrZUCHSO4D-UQgOUECK4O&amp;usg=AOvVaw3nyiYbgayHDvoYy9A255ZW</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>iphone 12 64gb azul + brinde</t>
+          <t>(seminovo) iphone 12 apple branco, 64gb</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>4249</v>
+        <v>3399.15</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://www.malibushop.com.br/apple/iphone-12-64gb-azul-brinde%3Fparceiro%3D1538%26srsltid%3DAd5pg_E96x-JS4agYEqHYrSoBjD0sZ_kWvk8yeKTs771E3NL3hMxzk4SINo&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjj1fvO2Of8AhU0q5UCHckxBVEQgOUECKMQ&amp;usg=AOvVaw3VVkCZeMoEugpi9_q2KTGa</t>
+          <t>https://www.google.com.br/url?url=https://www.taqi.com.br/seminovo-iphone-12-apple-branco-64gb/222815%3Fsrsltid%3DAd5pg_E1PaeDzHYSri90ZmmDkkaNrI9EMh5-oCtaiGTMMux1ggjJW-So47Y&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjpuMvd3uf8AhVOrZUCHSO4D-UQgOUECL0O&amp;usg=AOvVaw1taVhPTPNlTCr0lYew6RP_</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>iphone 12 lilás 64gb vitrine | celular apple | usado</t>
+          <t>(seminovos) iphone 12 apple azul, 64gb</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>4173</v>
+        <v>3399.15</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://www.enjoei.com.br/p/iphone-12-lilas-64gb-vitrine-72711813%3Fg_campaign%3Dgoogle_shopping&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjj1fvO2Of8AhU0q5UCHckxBVEQgOUECKoR&amp;usg=AOvVaw2W82BhNj-4wcYf1hcYdNxM</t>
+          <t>https://www.google.com.br/url?url=https://www.taqi.com.br/seminovo-iphone12-apple-azul64gb-nacional/220673%3Fsrsltid%3DAd5pg_Gnc2sL__MJVqEQ2uw3hhzCHW5BzxHmG3ySk6qBvJimRU8HZf9yW-I&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjpuMvd3uf8AhVOrZUCHSO4D-UQgOUECMwO&amp;usg=AOvVaw0P-74dR7TGY5YLaOZUZGJG</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>iphone 12 64 gb no pix r$ 3.040,00</t>
+          <t>smartphone apple iphone 12 - oled 6.1" 64/128/256gb ios 16 hexa 3.1ghz 12mp 4k ...</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>3800</v>
+        <v>3649.9</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://lojameusmart.com/index.php/produto/iphone-12-64-gb/%3Fattribute_pa_cor%3Dpreto&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjj1fvO2Of8AhU0q5UCHckxBVEQgOUECMoR&amp;usg=AOvVaw3BUc6kvfkwcwfjJfEBIVHq</t>
+          <t>https://www.google.com.br/url?url=https://www.rbaimportados.com/celulares/recondicionados-de-fabrica/iphone-12.html%3Ffee%3D2%26fep%3D1263&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjpuMvd3uf8AhVOrZUCHSO4D-UQgOUECNsO&amp;usg=AOvVaw19BqG8X3a2rCoHLA0EgvQP</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>vitrine: iphone 12 apple 64gb preto tela 6,1 câmera traseira dupla 12mp ios</t>
+          <t>(seminovos) iphone 12 apple branco, 64gb</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>4439</v>
+        <v>3519.12</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://www.kabum.com.br/produto/233224/iphone-12-apple-64gb-preto-tela-6-1-camera-traseira-dupla-12mp-ios-usado%3Fsrsltid%3DAd5pg_HHEQLO-YuNV_lZh3m4vDd6f0BMLHPADQvqe8qewPKCXF_F8Z559E0&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjj1fvO2Of8AhU0q5UCHckxBVEQguUECOwR&amp;usg=AOvVaw1UjfdBQ1d80GXqY-XmVRbL</t>
+          <t>https://www.google.com.br/url?url=https://www.taqi.com.br/seminovos-apple-iphone12-64gb/220684%3Fsrsltid%3DAd5pg_ETqrxUpovcL7MNaY_NpNpZT6pVZPntBHkUisIQZMvow_pxct-T5Qo&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjpuMvd3uf8AhVOrZUCHSO4D-UQgOUECJcP&amp;usg=AOvVaw36ZM-dzdzASRq4RO09z6vf</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>iphone 12 64gb verde seminovo</t>
+          <t>iphone 12 apple 64gb (product)red 6,1" - ios + microsoft 365 personal office 365 ...</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>2600</v>
+        <v>4478</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://loja.switchphone.com.br/iphone-12-64gb-verde-seminovo%3Fsrsltid%3DAd5pg_H2jBUtaGemBeJwszLDujmaHXMkbGpIZtrL0pJRajqeXff6rXmhDR4&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjj1fvO2Of8AhU0q5UCHckxBVEQgOUECMsS&amp;usg=AOvVaw0mWU9RVPCzlSdpnCZVk8yi</t>
+          <t>https://www.google.com.br/url?url=https://www.shoppingsmiles.com.br/smiles/produto.jsf%3Fs%3D2297537-00%26p%3D2297537_8%26a%3Dtrue&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjpuMvd3uf8AhVOrZUCHSO4D-UQgOUECLYP&amp;usg=AOvVaw3rhA-N2WQ4pVgVj6WDXxqM</t>
         </is>
       </c>
     </row>
@@ -731,112 +731,112 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://www.aproveiteiofertas.com.br/products/iphone-12-com-brinde-surpresa-da-aproveitei%3Fvariant%3D44152943903029%26currency%3DBRL%26utm_medium%3Dproduct_sync%26utm_source%3Dgoogle%26utm_content%3Dsag_organic%26utm_campaign%3Dsag_organic&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjj1fvO2Of8AhU0q5UCHckxBVEQgOUECOoS&amp;usg=AOvVaw1SehEXOorDSCmkuDNAMf2M</t>
+          <t>https://www.google.com.br/url?url=https://www.aproveiteiofertas.com.br/products/iphone-12-com-brinde-surpresa-da-aproveitei%3Fvariant%3D44152943903029%26currency%3DBRL%26utm_medium%3Dproduct_sync%26utm_source%3Dgoogle%26utm_content%3Dsag_organic%26utm_campaign%3Dsag_organic&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjpuMvd3uf8AhVOrZUCHSO4D-UQgOUECNMP&amp;usg=AOvVaw3LrXxkH_h8MUA2PGtUUtAa</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>iphone 12 64gb verde claro | celular apple</t>
+          <t>(seminovos) iphone 12 apple (product)red , 64gb</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>4215</v>
+        <v>3399.15</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://www.enjoei.com.br/p/iphone-12-64gb-verde-lacrado-com-garantia-80557246%3Fg_campaign%3Dgoogle_shopping&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjj1fvO2Of8AhU0q5UCHckxBVEQgOUECIgT&amp;usg=AOvVaw3kec7R1IWSCwJ7dSlMJaFt</t>
+          <t>https://www.google.com.br/url?url=https://www.taqi.com.br/seminovos-apple-iphone-12-64gb-productred/221656%3Fsrsltid%3DAd5pg_FgiAMSDZPXQmOrGSgmDs0cBk-XUOaHgLaVLWstoC0luw0cDOxznAw&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjpuMvd3uf8AhVOrZUCHSO4D-UQgOUECJ0Q&amp;usg=AOvVaw22kkbakZNio-l8GckP_hfv</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>iphone 12 64gb vermelho + brinde</t>
+          <t>iphone 12 64gb branco seminovo novinho</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>4249</v>
+        <v>3495</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://www.malibushop.com.br/apple/iphone-12-64gb-vermelho-brinde%3Fparceiro%3D1538%26srsltid%3DAd5pg_E2VK2hR21zXllstpwWRK_McWvnlqh7B48PG4ezVfLLUgrL2BGAI9A&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjj1fvO2Of8AhU0q5UCHckxBVEQgOUECJcT&amp;usg=AOvVaw15wDZ-zgZvTFtVOWWaHXu-</t>
+          <t>https://www.google.com.br/url?url=https://www.ztcompras.com/produtos/iphone-12-64gb-branco-seminovo-novinho/&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjpuMvd3uf8AhVOrZUCHSO4D-UQgOUECLwQ&amp;usg=AOvVaw3-dF6fGarWB6ib8FuK1TSg</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>iphone 12 64gb | celular iphone | usado</t>
+          <t>iphone xs max 64gb dourado câmera 12mp ios 12 4g</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>4015</v>
+        <v>2950</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://www.enjoei.com.br/p/iphone-12-64gb-78829276%3Fg_campaign%3Dgoogle_shopping&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjj1fvO2Of8AhU0q5UCHckxBVEQgOUECKYT&amp;usg=AOvVaw1hp8QGblN8X881cM7umhxB</t>
+          <t>https://www.google.com.br/url?url=https://www.mercadolivre.com.br/iphone-xs-max-64-gb-dourado/p/MLB12866628%3Fmatt_tool%3D18956390%26utm_source%3Dgoogle_shopping%26utm_medium%3Dorganic&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjpuMvd3uf8AhVOrZUCHSO4D-UQguUECMUR&amp;usg=AOvVaw2RAlkBYrTgPbj4obQLISOC</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>smartphone apple iphone 12 64gb câmera dupla</t>
+          <t>iphone 12 64 gb no pix r$ 3.040,00</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>4064.09</v>
+        <v>3800</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>https://www.buscape.com.br/celular/smartphone-apple-iphone-12-64gb-ios?_lc=88&amp;searchterm=iphone%2012%2064%20gb</t>
+          <t>https://www.google.com.br/url?url=https://lojameusmart.com/index.php/produto/iphone-12-64-gb/%3Fattribute_pa_cor%3Dpreto&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjpuMvd3uf8AhVOrZUCHSO4D-UQgOUECIQS&amp;usg=AOvVaw2hLYg7MDgyIRlwotSY0LcY</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>smartphone apple iphone 12 vermelho 64gb câmera dupla</t>
+          <t>smartphone apple iphone 12 64gb câmera dupla</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>3999</v>
+        <v>4123</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>https://www.buscape.com.br/celular/smartphone-apple-iphone-12-vermelho-64gb-ios?_lc=88&amp;searchterm=iphone%2012%2064%20gb</t>
+          <t>https://www.buscape.com.br/celular/smartphone-apple-iphone-12-64gb-ios?_lc=88&amp;searchterm=iphone%2012%2064%20gb</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>placa de video colorful igame geforce rtx 3060 nb duo lhr-v 12gb gddr6 192bit</t>
+          <t>smartphone apple iphone 12 vermelho 64gb câmera dupla</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>2594.67</v>
+        <v>3999</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://www.casasbahia.com.br/placa-de-video-colorful-igame-geforce-rtx-3060-nb-duo-lhr-v-12gb-gddr6-192bit-1535388927/p/1535388927%3Futm_medium%3DCpc%26utm_source%3Dgoogle_freelisting%26IdSku%3D1535388927%26idLojista%3D22088%26tipoLojista%3D3P&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiK3JHT2Of8AhVXq5UCHUbYArcQguUECMAN&amp;usg=AOvVaw0In9aHLjoUSloIa2tiLX8J</t>
+          <t>https://www.buscape.com.br/celular/smartphone-apple-iphone-12-vermelho-64gb-ios?_lc=88&amp;searchterm=iphone%2012%2064%20gb</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>placa de vídeo msi nvidia rtx 3060 12gb gddr6 gaming z trio</t>
+          <t>placa de video colorful igame geforce rtx 3060 nb duo lhr-v 12gb gddr6 192bit</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>3402.97</v>
+        <v>2594.67</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://www.bitboss.com.br/padrao/gpu-nv-rtx3060-12gb-gddr6-gaming-z-trio-oc-msi-912-v390-245%3Fparceiro%3D4465%26srsltid%3DAd5pg_HH439mcOV_5gWHP3CQkYrH9ffhR3ecsrWxXv8ksd8w4ERuYUWPRvM&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiK3JHT2Of8AhVXq5UCHUbYArcQguUECPIN&amp;usg=AOvVaw3-Kb6Ri7cR9_Xgzfkj2C9P</t>
+          <t>https://www.google.com.br/url?url=https://www.casasbahia.com.br/placa-de-video-colorful-igame-geforce-rtx-3060-nb-duo-lhr-v-12gb-gddr6-192bit-1535388927/p/1535388927%3Futm_medium%3DCpc%26utm_source%3Dgoogle_freelisting%26IdSku%3D1535388927%26idLojista%3D22088%26tipoLojista%3D3P&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjRuOPh3uf8AhWWpZUCHZV_BscQguUECM0L&amp;usg=AOvVaw3m1MLo0H1XYaTIH9BFL53g</t>
         </is>
       </c>
     </row>
@@ -847,624 +847,354 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>3364.39</v>
+        <v>2760.38</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://www.mercadolivre.com.br/placa-de-video-nvidia-asus-dual-geforce-rtx-30-series-rtx-3060-dual-rtx3060-o12g-v2-oc-edition-12gb/p/MLB18761117%3Fmatt_tool%3D18956390%26utm_source%3Dgoogle_shopping%26utm_medium%3Dorganic&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiK3JHT2Of8AhVXq5UCHUbYArcQguUECIMO&amp;usg=AOvVaw16rrHQn9dQtG4QtQozgyoB</t>
+          <t>https://www.google.com.br/url?url=https://www.chipart.com.br/placa-de-video-pci-e-12gb-gddr6-asus-rtx-3060-dual&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjRuOPh3uf8AhWWpZUCHZV_BscQguUECO0L&amp;usg=AOvVaw1WqFEqRnXBAolKo5vvtXrv</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>placa de vídeo msi nvidia geforce rtx 3060 ventus 2x oc, lhr, 8gb gddr6, dlss ...</t>
+          <t>placa de vídeo nvidia geforce rtx 3060 verto 12gb gddr6 pny</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>2589</v>
+        <v>3058.24</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://www.terabyteshop.com.br/produto/20438/placa-de-video-msi-geforce-rtx-3060-ventus-2x-oc-lhr-12gb-gddr6-dlss-ray-tracing-912-v397-050%3Fsrsltid%3DAd5pg_H5o0uIyvg895LT9rHKuEtrbs1vDaG--N3qvlO28whkAO0ixonghXg&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiK3JHT2Of8AhVXq5UCHUbYArcQgOUECKUO&amp;usg=AOvVaw1rJbRDqMVWNE28MjIRnKtI</t>
+          <t>https://www.google.com.br/url?url=https://www.bitboss.com.br/padrao/gpu-nv-rtx3060-12gb-g6-192b-verto-pny-vcg306012dfbpb1%3Fparceiro%3D4465%26srsltid%3DAd5pg_GK4RPr8OANMzsr3vfT_LrxpazPTzT8f3o272JiYvfK2Ah1CNz1Tm4&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjRuOPh3uf8AhWWpZUCHZV_BscQguUECI0M&amp;usg=AOvVaw23c4DvTqhfvydrhFnO1jsz</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>placa de vídeo nvidia geforce rtx 3060 verto 12gb gddr6 pny</t>
+          <t>placa de vídeo palit geforce rtx 3060 12gb - gddr6 dual ne63060019k9-190ad</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>3319.9</v>
+        <v>2559</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://www.pontofrio.com.br/placa-de-video-nvidia-geforce-rtx-3060-verto-pny-12gb-gddr6-192bits-vcg306012dfbpb1-1554225523/p/1554225523%3Futm_medium%3Dcpc%26utm_source%3Dgoogle_freelisting%26IdSku%3D1554225523%26idLojista%3D207611%26tipoLojista%3D3P&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiK3JHT2Of8AhVXq5UCHUbYArcQguUECMUO&amp;usg=AOvVaw0ZDkweSgaNk6NYWwMhXoWH</t>
+          <t>https://www.google.com.br/url?url=https://www.terabyteshop.com.br/produto/17611/placa-de-video-palit-nvidia-geforce-rtx-3060-dual-12gb-gddr6-192bit-ne63060019k9-190ad%3Fsrsltid%3DAd5pg_HS831yFh45Cvc3_LH_JgMjykxA1vLuWCKBuSTqaLGxbgQzf8BAw48&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjRuOPh3uf8AhWWpZUCHZV_BscQguUECLcM&amp;usg=AOvVaw2EurXGmYhcraBL3vaFXPX2</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>placa de vídeo asus geforce tuf gaming rtx 3060 12gb v2</t>
+          <t>yeston gddr6 nvidia rtx 3060 graphic card 12g gaming gpu video cards rgb rtx3060 ...</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>3168.92</v>
+        <v>2566.36</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://www.bringit.com.br/placa-de-video-asus-nvidia-geforce-rtx-3060-v2-oc-edition-12gb-gddr6-lhr-192-bits-hdmi-dp-tuf-rtx3060-o12g-v2-gaming.html%3Fsrsltid%3DAd5pg_GWN3pTcbSNvxJE74fu0jNa2sWO-hbG9rlVYpdNusTgXdR0DbV_N3g&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiK3JHT2Of8AhVXq5UCHUbYArcQguUECNYO&amp;usg=AOvVaw09Ch0iE2S3BAiNYBjTqITt</t>
+          <t>https://www.google.com.br/url?url=https://s.click.aliexpress.com/deep_link.htm%3Faff_short_key%3DUneMJZVf%26dl_target_url%3Dhttps%253A%252F%252Fpt.aliexpress.com%252Fitem%252F1005004678434448.html%253F_randl_currency%253DBRL%2526_randl_shipto%253DBR%2526src%253Dgoogle&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjRuOPh3uf8AhWWpZUCHZV_BscQgOUECNgO&amp;usg=AOvVaw073u-SxcA--ySITeSQhAM8</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>placa de vídeo colorful igame geforce rtx 3060 mini 192bit</t>
+          <t>yeston rtx3060-12g d6 lb tarjeta gráfica 192bit / gddr6 tarjetas de video modo de ...</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>2879</v>
+        <v>2806.49</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://www.americanas.com.br/produto/4796211460%3Fopn%3DYSMESP%26offerId%3D62ac06b32376eb9c728af832%26srsltid%3DAd5pg_EJoAAmBu45PY7gCDLxIQxueVGyViJXq-bB9-RCiJ3nJvaXo4M5028&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiK3JHT2Of8AhVXq5UCHUbYArcQguUECOUO&amp;usg=AOvVaw1Toarp-LTD4dGTQnSgsft9</t>
+          <t>https://www.google.com.br/url?url=https://s.click.aliexpress.com/deep_link.htm%3Faff_short_key%3DUneMJZVf%26dl_target_url%3Dhttps%253A%252F%252Fpt.aliexpress.com%252Fitem%252F1005004272882225.html%253F_randl_currency%253DBRL%2526_randl_shipto%253DBR%2526src%253Dgoogle&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjRuOPh3uf8AhWWpZUCHZV_BscQgOUECOQO&amp;usg=AOvVaw0ddhvQkemQamCVwHbKLan7</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>placa de vídeo, gigabyte, geforce rtx 3060 vision oc 12g lhr, gddr6, dlss ray ...</t>
+          <t>yeston geforce rtx3060 graphics cards amd radeon rx6700xt rx6800 16g rx6800xt gpu ...</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>2699.99</v>
+        <v>2598.8</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://www.kabum.com.br/produto/150631/placa-de-video-rtx-3060-vision-oc-12g-gigabyte-geforce-12gb-gddr6-rgb-fusion-ray-tracing-metal-back-plate-gv-n3060vision-oc-12gd%3Fsrsltid%3DAd5pg_HQVpi8nmvYA7W9T6OVgsq5aRVqriQFVaCFAL_VBdHcuRl-goz_oFo&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiK3JHT2Of8AhVXq5UCHUbYArcQguUECIIP&amp;usg=AOvVaw3fzrkk_4WXCu1SD8-vaJps</t>
+          <t>https://www.google.com.br/url?url=https://s.click.aliexpress.com/deep_link.htm%3Faff_short_key%3DUneMJZVf%26dl_target_url%3Dhttps%253A%252F%252Fpt.aliexpress.com%252Fitem%252F1005004360564341.html%253F_randl_currency%253DBRL%2526_randl_shipto%253DBR%2526src%253Dgoogle&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjRuOPh3uf8AhWWpZUCHZV_BscQgOUECO8O&amp;usg=AOvVaw0PpIXN3pyMKprtVjxQzq4Q</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>placa de vídeo msi rtx 3060ti twin fan oc edition 8gb</t>
+          <t>yeston rtx3060-12g d6 lb tarjeta gráfica para juegos 12g/192bit/gddr6 memoria ...</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>2999</v>
+        <v>2885.98</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://www.terabyteshop.com.br/produto/21586/placa-de-video-msi-nvidia-geforce-rtx-3060-ti-twin-fan-8g-oc-lhr-gddr6-dlss-ray-tracing%3Fsrsltid%3DAd5pg_EFPTluzye2VtoISBz048fjZnFAR05baW7IkNVWgLyJcnADKVdAmrk&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiK3JHT2Of8AhVXq5UCHUbYArcQguUECJEP&amp;usg=AOvVaw16gDqc58MPaqpe3jie6NTD</t>
+          <t>https://www.google.com.br/url?url=https://s.click.aliexpress.com/deep_link.htm%3Faff_short_key%3DUneMJZVf%26dl_target_url%3Dhttps%253A%252F%252Fpt.aliexpress.com%252Fitem%252F1005004272889143.html%253F_randl_currency%253DBRL%2526_randl_shipto%253DBR%2526src%253Dgoogle&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjRuOPh3uf8AhWWpZUCHZV_BscQgOUECIgP&amp;usg=AOvVaw2M6WcyK_7xjfwoj0Sj_FQw</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>placa de vdeo rtx 3060 huananzhi 12gb msi</t>
+          <t>yeston nvidia geforce rtx 3060ti placa gráfica gddr6 8 gb 256 bit rgb placa de ...</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>2500</v>
+        <v>2851.7</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://produto.mercadolivre.com.br/MLB-3050168867-placa-de-video-rtx3060-12gb-huananzhi-_JM%3Fmatt_tool%3D18956390%26utm_source%3Dgoogle_shopping%26utm_medium%3Dorganic&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiK3JHT2Of8AhVXq5UCHUbYArcQguUECLAP&amp;usg=AOvVaw2ckLR9QNfVLpBMzqC6EQkt</t>
+          <t>https://www.google.com.br/url?url=https://s.click.aliexpress.com/deep_link.htm%3Faff_short_key%3DUneMJZVf%26dl_target_url%3Dhttps%253A%252F%252Fpt.aliexpress.com%252Fitem%252F1005004504718650.html%253F_randl_currency%253DBRL%2526_randl_shipto%253DBR%2526src%253Dgoogle%2526memo1%253Dfreelisting&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjRuOPh3uf8AhWWpZUCHZV_BscQgOUECMsP&amp;usg=AOvVaw0WKyLa_yMhNbyzjkZLb-Su</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>placa de vídeo gainward geforce rtx 3060 pegasus 12gb gddr6</t>
+          <t>yeston rtx3060-12g d6 gaming placa gráfica 192bit gddr6 15gbps interface de saída ...</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>2668</v>
+        <v>2519.66</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://www.carrefour.com.br/placa-de-video-12gb-rtx3060-ddr6-192bit-hdmi3xdisplayport-rtx3060-pegasus-gainward-mp927925967/p&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiK3JHT2Of8AhVXq5UCHUbYArcQguUECM4P&amp;usg=AOvVaw1ZeSikyNVQ1YYVsXmubQNs</t>
+          <t>https://www.google.com.br/url?url=https://s.click.aliexpress.com/deep_link.htm%3Faff_short_key%3DUneMJZVf%26dl_target_url%3Dhttps%253A%252F%252Fpt.aliexpress.com%252Fitem%252F1005004660983072.html%253F_randl_currency%253DBRL%2526_randl_shipto%253DBR%2526src%253Dgoogle&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjRuOPh3uf8AhWWpZUCHZV_BscQgOUECOcP&amp;usg=AOvVaw1Sl2baRk9UcXDnVFGBEpBF</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>placa de video colorful igame geforce rtx 3060 ultra w oc lhr-v 12gb gddr6 192bit</t>
+          <t>yeston geforce rtx 3060ti nvidia placa gráfica jogos 8gb gddr6 256bit 14000mhz ...</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>2659.05</v>
+        <v>2656.95</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://produto.mercadolivre.com.br/MLB-2171962853-placa-video-colorful-geforce-rtx-3060-ultra-w-oc-lhr-12gb-_JM%3Fmatt_tool%3D18956390%26utm_source%3Dgoogle_shopping%26utm_medium%3Dorganic&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiK3JHT2Of8AhVXq5UCHUbYArcQguUECOsP&amp;usg=AOvVaw1O7wamINHtXsiZmnown3Ct</t>
+          <t>https://www.google.com.br/url?url=https://s.click.aliexpress.com/deep_link.htm%3Faff_short_key%3DUneMJZVf%26dl_target_url%3Dhttps%253A%252F%252Fpt.aliexpress.com%252Fitem%252F1005004630423498.html%253F_randl_currency%253DBRL%2526_randl_shipto%253DBR%2526src%253Dgoogle&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjRuOPh3uf8AhWWpZUCHZV_BscQgOUECIMQ&amp;usg=AOvVaw09sHbEjGmFybyhiVT2XO0u</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>placa de video asus geforce rtx 3060 ti dual oc, lhr, 8gb gddr6, 256bit, dual ...</t>
+          <t>maxsun rtx 3060ti terminator placas gráficas 8g gddr6 gpu computador pc gaming ...</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>3191.99</v>
+        <v>2524.08</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://www.fantasygaming.com.br/placa-de-video-asus-geforce-rtx-3060-ti-dual-v2-oc-edition-rgb-8gb-gddr6-lhr-256bit%3Futm_source%3DSite%26utm_medium%3DGoogleMerchant%26utm_campaign%3DGoogleMerchant&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiK3JHT2Of8AhVXq5UCHUbYArcQguUECPsP&amp;usg=AOvVaw2Ilur1K45HfspM7lFdeS6q</t>
+          <t>https://www.google.com.br/url?url=https://s.click.aliexpress.com/deep_link.htm%3Faff_short_key%3DUneMJZVf%26dl_target_url%3Dhttps%253A%252F%252Fpt.aliexpress.com%252Fitem%252F1005004299978839.html%253F_randl_currency%253DBRL%2526_randl_shipto%253DBR%2526src%253Dgoogle&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjRuOPh3uf8AhWWpZUCHZV_BscQgOUECI8Q&amp;usg=AOvVaw1Hvdm6eYBo9YX_q-jU_i9G</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>placa de video asus geforce rtx 3060 dual oc, 8gb, gddr6, 128-bit, dual-rtx3060-o8g</t>
+          <t>maxsun placas gráficas geforce rtx 3060ti icraft oc 8g gddr6 gpu 8nm nvidia ...</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>3129.99</v>
+        <v>2646.56</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://www.kabum.com.br/produto/398081/placa-de-video-rtx-3060-oc-edition-asus-dual-geforce-8-gb-gddr6-dlss-ray-tracing-dual-rtx3060-o8g%3Fsrsltid%3DAd5pg_E2Stu0bBrgammVfZfqw10VaBFM4x1LeSqEwOa9ln8LX6eJ7kbkoJU&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiK3JHT2Of8AhVXq5UCHUbYArcQguUECIwQ&amp;usg=AOvVaw1d6Ony3BYN0IPNK_bG1lM5</t>
+          <t>https://www.google.com.br/url?url=https://s.click.aliexpress.com/deep_link.htm%3Faff_short_key%3DUneMJZVf%26dl_target_url%3Dhttps%253A%252F%252Fpt.aliexpress.com%252Fitem%252F1005004623072723.html%253F_randl_currency%253DBRL%2526_randl_shipto%253DBR%2526src%253Dgoogle%2526memo1%253Dfreelisting&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjRuOPh3uf8AhWWpZUCHZV_BscQgOUECKsQ&amp;usg=AOvVaw3rmQX9ffdOtsfDQljm8sXf</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>placa de video msi geforce rtx 3060 gaming x 12gb gddr6 192</t>
+          <t>yeston nueva tarjeta gráfica rtx 3060 12g 12gb gddr6 geforce tarjeta de video ...</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>3699</v>
+        <v>2725.43</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://www.shoptime.com.br/produto/5316223438%3Fopn%3DGOOGLEXML%26offerId%3D62b1e053f2adc6d985f650d4%26srsltid%3DAd5pg_GpVj-nTbDB_z6NIgR72t9GzrOmit89_WL-HCqu2yDhUKNaU2SqB_8&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiK3JHT2Of8AhVXq5UCHUbYArcQguUECJ0Q&amp;usg=AOvVaw2s3hF7-4WoM06wxozpvwIk</t>
+          <t>https://www.google.com.br/url?url=https://s.click.aliexpress.com/deep_link.htm%3Faff_short_key%3DUneMJZVf%26dl_target_url%3Dhttps%253A%252F%252Fpt.aliexpress.com%252Fitem%252F1005004500651157.html%253F_randl_currency%253DBRL%2526_randl_shipto%253DBR%2526src%253Dgoogle&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjRuOPh3uf8AhWWpZUCHZV_BscQgOUECLcQ&amp;usg=AOvVaw3lYBYDRANkN1FMsFCGW6TP</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>placa de video msi geforce rtx 3060 ti gaming x, lhr, 8gb, gddr6, 256-bit, 912 ...</t>
+          <t>placa de video nvidia geforce rtx 3060 12 gb gddr6 192 bits palit ne63060019k9-190ad</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>3299.99</v>
+        <v>2849</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://www.pichau.com.br/placa-de-video-msi-geforce-rtx-3060-ti-gaming-x-lhr-8gb-gddr6-256-bit-912-v397-234&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiK3JHT2Of8AhVXq5UCHUbYArcQguUECL4Q&amp;usg=AOvVaw1XlFCGLEjv_9DfvsdJJU-X</t>
+          <t>https://www.buscape.com.br/placa-de-video/placa-de-video-nvidia-geforce-rtx-3060-12-gb-gddr6-192-bits-palit-ne63060019k9-190ad?_lc=88&amp;searchterm=rtx%203060</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>placa de vídeo rtx 3060 white oc edition asus nvidia dual geforce, 8 gb gddr6 ...</t>
+          <t>placa de video nvidia geforce rtx 3060 ti 8 gb gddr6 256 bits gainward ne6306t019p2-190ab v1</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>2699.99</v>
+        <v>3299</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://www.kabum.com.br/produto/398083/placa-de-video-rtx-3060-white-oc-edition-asus-nvidia-dual-geforce-8-gb-gddr6-dlss-ray-tracing-dual-rtx3060-o8g-white%3Fsrsltid%3DAd5pg_HqQib5IL-zIfNHHr0XQHgPt5aPC0HCooWFgDtdh8JJizNXtHU3gMk&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiK3JHT2Of8AhVXq5UCHUbYArcQguUECIQR&amp;usg=AOvVaw0xifZv0Uh07ACGRp0FEjG1</t>
+          <t>https://www.buscape.com.br/placa-de-video/placa-de-video-nvidia-geforce-rtx-3060-ti-8-gb-gddr6-256-bits-gainward-ne6306t019p2-190ab-v1?_lc=88&amp;searchterm=rtx%203060</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>placa de video pny geforce rtx 3060 ti xlr8 gaming epic-x rgb lhr, 8gb, gddr6 ...</t>
+          <t>placa de video nvidia geforce rtx 3060 12 gb gddr6 192 bits gainward ne63060019k9-190au</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>3149.1</v>
+        <v>2999</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://www.r2computadores.com.br/placa-de-video-geforce-rtx-3060-ti-8gb-pny-vcg3060t8ldfxppb1-3355%3Fparceiro%3D7445&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiK3JHT2Of8AhVXq5UCHUbYArcQguUECKMR&amp;usg=AOvVaw3TPTryJlDam1i0TO2_Xk4O</t>
+          <t>https://www.buscape.com.br/placa-de-video/placa-de-video-nvidia-geforce-rtx-3060-12-gb-gddr6-192-bits-gainward-ne63060019k9-190au?_lc=88&amp;searchterm=rtx%203060</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>placa de vídeo pny rtx 3060 12gb gddr6 revel epic-x</t>
+          <t>pny placa gráfica geforce rtx™ 3060 ti 8gb xlr8 gaming revel epic-x rgb™ dual fan lhr</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>2759.99</v>
+        <v>3264.9</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://www.kabum.com.br/produto/335122/placa-de-video-rtx-3060-12gb-epic-pny-geforce-rgb-12gb-gddr6-lhr-nvidia-dlss-ray-tracing-dual-fan-nvidia-g-sync-vcg306012dfxppb%3Fsrsltid%3DAd5pg_E16sUHBJmX8TRgYd28Y9rw8XgS2EFP6vZP7g3ynvALKF7CuI0OO1w&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiK3JHT2Of8AhVXq5UCHUbYArcQguUECLQR&amp;usg=AOvVaw3L4RzznbpV9BvHtaM--bsy</t>
+          <t>https://www.buscape.com.br/lead?oid=558532017&amp;channel=86&amp;index=6&amp;searchterm=rtx%203060</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>placa de vídeo asus gaming - geforce dual rtx 3060, 12gb gddr6, rgb, lhr, ray ...</t>
+          <t>placa de vídeo rtx 3060 gaming z trio msi nvidia geforce, 12gb gddr, rgb, dlss, ray tracing</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>2599.99</v>
+        <v>2799.99</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://www.amazon.com.br/Placa-V%25C3%25ADdeo-ASUS-TUF-Gaming/dp/B096658ZWP%3Fsource%3Dps-sl-shoppingads-lpcontext%26ref_%3Dfplfs%26psc%3D1%26smid%3DA1ZZFT5FULY4LN&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiK3JHT2Of8AhVXq5UCHUbYArcQguUECPYR&amp;usg=AOvVaw11O78k9LwsZsJlFw4NsqSM</t>
+          <t>https://www.buscape.com.br/lead?oid=893145377&amp;channel=86&amp;index=8&amp;searchterm=rtx%203060</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>placa de vídeo palit geforce rtx 3060 ti lhr dual 8gb gddr6</t>
+          <t>placa de vídeo rtx 3060 ti pny nvidia geforce, 8gb xlr8, gaming revel epic, rgb, dual fan - vcg3060t8ldfxppb1</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>3136.44</v>
+        <v>3205.99</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://www.apriretech.com/MLB-3136952287-placa-de-video-nvidia-palit-dual-geforce-rtx-30-series-rtx-3060-ti-ne6306t019p2-190ad-8gb-_JM&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiK3JHT2Of8AhVXq5UCHUbYArcQguUECIUS&amp;usg=AOvVaw0XMxXVO4l-yayzNjXFRZnk</t>
+          <t>https://www.buscape.com.br/lead?oid=902491304&amp;channel=86&amp;index=9&amp;searchterm=rtx%203060</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>placa de vídeo rtx 3060 ti 3070 3080 3090 * consulte * leia nvidia</t>
+          <t>placa de vídeo rtx 3060 ti dual o8g v2 asus nvidia geforce, 8gb gddr6, rgb, dlss, lhr, ray tracing - dual-rtx3060ti-o8g-v2</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>4395</v>
+        <v>3299.99</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://produto.mercadolivre.com.br/MLB-1271524438-placa-de-video-rtx-3060-ti-3070-3080-3090-consulte-leia-_JM%3Fmatt_tool%3D18956390%26utm_source%3Dgoogle_shopping%26utm_medium%3Dorganic&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiK3JHT2Of8AhVXq5UCHUbYArcQgOUECJQS&amp;usg=AOvVaw0Y7FVbLV_Ic9f5R5K-8YrH</t>
+          <t>https://www.buscape.com.br/lead?oid=739872414&amp;channel=86&amp;index=10&amp;searchterm=rtx%203060</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>inno3d novo geforce rtx 3060 jogos 8g 12g 192 256bit nvidia gddr6 placas de vídeo ...</t>
+          <t>placa de vídeo rtx 3060 asus dual o12g v2 nvidia geforce, 12gb gddr6, lhr, dlss, ray tracing - dual-rtx3060-o12g-v2</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>2513.43</v>
+        <v>2599.99</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://s.click.aliexpress.com/deep_link.htm%3Faff_short_key%3DUneMJZVf%26dl_target_url%3Dhttps%253A%252F%252Fpt.aliexpress.com%252Fitem%252F1005004697964375.html%253F_randl_currency%253DBRL%2526_randl_shipto%253DBR%2526src%253Dgoogle&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiK3JHT2Of8AhVXq5UCHUbYArcQgOUECKIS&amp;usg=AOvVaw1L5ogBLOZdC916ZgwyYQut</t>
+          <t>https://www.buscape.com.br/lead?oid=699424736&amp;channel=86&amp;index=12&amp;searchterm=rtx%203060</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>msi placa gráfica rtx 3060 ti ventus oc lhr 8gb gddr6 prateado 1345751</t>
+          <t>gigabyte placa de vídeo geforce rtx 3060 gaming oc 12g (rev2.0), 3x ventiladores windforce 12gb 192-bit gddr6, gv-n3060gaming oc-12gd rev2.0</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>2999</v>
+        <v>4499</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://www.pichau.com.br/placa-de-video-msi-geforce-rtx-3060-ti-ventus-3x-oc-lhr-8gb-gddr6-256-bit-912-v397-246&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiK3JHT2Of8AhVXq5UCHUbYArcQguUECLQS&amp;usg=AOvVaw3YIXhg-VxbVf6pKmE8_5Zp</t>
+          <t>https://www.buscape.com.br/lead?oid=546338771&amp;channel=86&amp;index=13&amp;searchterm=rtx%203060</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>placa de vídeo palit geforce rtx 3060 dual oc 12gb gddr6</t>
+          <t>placa de vídeo rtx 3060 o12g v2 gaming asus tuf, 12gb gddr6, rgb, lhr, dlss, ray tracing - tuf-rtx3060-o12g-v2-gaming</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>3137.98</v>
+        <v>3399.99</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://www.americanas.com.br/produto/3492455326%3Fopn%3DYSMESP%26offerId%3D630924079064f2befb65e6d3%26srsltid%3DAd5pg_Esc8Cwv0H6RQ_mFvEcCtbFACk1CUzmpAF4an5uVXH_ml8aB9Q_4IA&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiK3JHT2Of8AhVXq5UCHUbYArcQguUECMQS&amp;usg=AOvVaw18-evs-v01Zj91z_NRu_D7</t>
+          <t>https://www.buscape.com.br/lead?oid=834707329&amp;channel=86&amp;index=14&amp;searchterm=rtx%203060</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>geforce rtx 3060 ventus 2x 12g oc - box(nacional) msi nvidia geforce rtx 3060 ti1 ...</t>
+          <t>placa de vídeo asus gaming - geforce dual rtx 3060, 12gb gddr6, rgb, lhr, ray tracing, dlss</t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>2887.75</v>
+        <v>3058.81</v>
       </c>
       <c r="C51" t="inlineStr">
-        <is>
-          <t>https://www.google.com.br/url?url=https://shopee.com.br/product/317501313/19964289274&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiK3JHT2Of8AhVXq5UCHUbYArcQgOUECNQS&amp;usg=AOvVaw0Zy3bq5MIrYZk2UJ1PXge7</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>processador grafico msi geforce912-v397-484 (gpu rtx 3060 ventus 2x 12gb gddr6)</t>
-        </is>
-      </c>
-      <c r="B52" t="n">
-        <v>2539.96</v>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>https://www.google.com.br/url?url=https://www.amazon.com.br/PROCESSADOR-GRAFICO-MSI-GEFORCE912-V397-484-VENTUS/dp/B08WHJFYM8%3Fsource%3Dps-sl-shoppingads-lpcontext%26ref_%3Dfplfs%26psc%3D1%26smid%3DA1ZZFT5FULY4LN&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiK3JHT2Of8AhVXq5UCHUbYArcQguUECPIS&amp;usg=AOvVaw0OrvAqFVMcZ0ZwpCD0Z9Kb</t>
-        </is>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>placa de video gigabyte geforce rtx 3060 ti vision 8gb lhr</t>
-        </is>
-      </c>
-      <c r="B53" t="n">
-        <v>2990.99</v>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>https://www.google.com.br/url?url=https://www.tradeinn.com/techinn/pt/gigabyte-placa-grafica-rtx-3060-ti-vision-oc-lhr-8gb-gddr6/138575822/p%3Futm_source%3Dgoogle_products%26utm_medium%3Dmerchant%26id_producte%3D15015516%26country%3Dbr&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiK3JHT2Of8AhVXq5UCHUbYArcQguUECI8T&amp;usg=AOvVaw1bGll0nR-h_jQy0iwHSb2Z</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>placa de video pci-e 12gb gddr6 asus tuf rtx 3060 v2 oc</t>
-        </is>
-      </c>
-      <c r="B54" t="n">
-        <v>2800.4</v>
-      </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>https://www.google.com.br/url?url=https://www.chipart.com.br/placa-de-video-pci-e-12gb-gddr6-asus-tuf-rtx-3060-v2-oc&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiK3JHT2Of8AhVXq5UCHUbYArcQgOUECMwT&amp;usg=AOvVaw1g1vO9EctR_dE2tA82NAVp</t>
-        </is>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>placa de vídeo nvidia msi geforce rtx 3060 ventus 3x 12g oc</t>
-        </is>
-      </c>
-      <c r="B55" t="n">
-        <v>2699</v>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>https://www.google.com.br/url?url=https://www.eliteplayer.com.br/placa-de-video-msi-geforce-rtx-3060-ventus-3x-oc-12gb-gddr6-192-bit-912-v397-051%3Fsrsltid%3DAd5pg_Fd5jFeLyqj4Lk0VryihaWEqBw6daPOvH9N69nEWaCj4Cvj-XaiS7E&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiK3JHT2Of8AhVXq5UCHUbYArcQguUECNwT&amp;usg=AOvVaw0odj01jMYWTJO7uvEeaxXr</t>
-        </is>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>placa de vídeo gainward geforce rtx 3060 ti 8gb ghost gddr6 - ne6306t019p2-190ab</t>
-        </is>
-      </c>
-      <c r="B56" t="n">
-        <v>2918.46</v>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>https://www.google.com.br/url?url=https://patoloco.com.br/placa-de-video-gainward-geforce-rtx-3060-ti-ghost-8gb-gddr6-256bits-ne6306t019p2-190ab-lhr&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiK3JHT2Of8AhVXq5UCHUbYArcQguUECJcU&amp;usg=AOvVaw15sqoQzHDDsT4mR9JdTp9X</t>
-        </is>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>msi geforce rtx 3060 ti ventus 3x 8g oc lhr - placa gráfica - gf rtx 3060 ti - 8 ...</t>
-        </is>
-      </c>
-      <c r="B57" t="n">
-        <v>3499.99</v>
-      </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>https://www.google.com.br/url?url=https://www.magazineluiza.com.br/placa-de-video-rtx-3060-ti-ventus-3x-oc-msi-nvidia-geforce-8gb-lhr-dlss-ray-tracing/p/ek9ckeff3c/in/pcvd/%3F%26seller_id%3Dkabum&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiK3JHT2Of8AhVXq5UCHUbYArcQguUECKgU&amp;usg=AOvVaw3KaZtDydHNl6WXtU5b1yOl</t>
-        </is>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>pc gamer u3, ryzen 5 5600g, geforce rtx 3060, 8gb ddr4, 240gb ssd nvme, gabinete ...</t>
-        </is>
-      </c>
-      <c r="B58" t="n">
-        <v>4399.89</v>
-      </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>https://www.google.com.br/url?url=https://www.lojanovaera.com/produto/pc-gamer-u5-ryzen-5-5600g-geforce-rtx-3060-8gb-ddr4-ssd-240gb-gabinete-lateral-de-vidro.html%3Futm_source%3DSite%26utm_medium%3DGoogleMerchant%26utm_campaign%3DGoogleMerchant&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiK3JHT2Of8AhVXq5UCHUbYArcQgOUECLYU&amp;usg=AOvVaw2eEb4MStFhEnJlByosv4GQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>placa de video nvidia geforce rtx 3060 12 gb gddr6 192 bits palit ne63060019k9-190ad</t>
-        </is>
-      </c>
-      <c r="B59" t="n">
-        <v>2849</v>
-      </c>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>https://www.buscape.com.br/placa-de-video/placa-de-video-nvidia-geforce-rtx-3060-12-gb-gddr6-192-bits-palit-ne63060019k9-190ad?_lc=88&amp;searchterm=rtx%203060</t>
-        </is>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="inlineStr">
-        <is>
-          <t>placa de video nvidia geforce rtx 3060 ti 8 gb gddr6 256 bits gainward ne6306t019p2-190ab v1</t>
-        </is>
-      </c>
-      <c r="B60" t="n">
-        <v>3299</v>
-      </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>https://www.buscape.com.br/placa-de-video/placa-de-video-nvidia-geforce-rtx-3060-ti-8-gb-gddr6-256-bits-gainward-ne6306t019p2-190ab-v1?_lc=88&amp;searchterm=rtx%203060</t>
-        </is>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>placa de video nvidia geforce rtx 3060 12 gb gddr6 192 bits gainward ne63060019k9-190au</t>
-        </is>
-      </c>
-      <c r="B61" t="n">
-        <v>2999</v>
-      </c>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t>https://www.buscape.com.br/placa-de-video/placa-de-video-nvidia-geforce-rtx-3060-12-gb-gddr6-192-bits-gainward-ne63060019k9-190au?_lc=88&amp;searchterm=rtx%203060</t>
-        </is>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>pny placa gráfica geforce rtx™ 3060 ti 8gb xlr8 gaming revel epic-x rgb™ dual fan lhr</t>
-        </is>
-      </c>
-      <c r="B62" t="n">
-        <v>3264.9</v>
-      </c>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t>https://www.buscape.com.br/lead?oid=558532017&amp;channel=86&amp;index=6&amp;searchterm=rtx%203060</t>
-        </is>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="inlineStr">
-        <is>
-          <t>placa de vídeo rtx 3060 gaming z trio msi nvidia geforce, 12gb gddr, rgb, dlss, ray tracing</t>
-        </is>
-      </c>
-      <c r="B63" t="n">
-        <v>2799.99</v>
-      </c>
-      <c r="C63" t="inlineStr">
-        <is>
-          <t>https://www.buscape.com.br/lead?oid=893145377&amp;channel=86&amp;index=8&amp;searchterm=rtx%203060</t>
-        </is>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="inlineStr">
-        <is>
-          <t>placa de vídeo rtx 3060 ti pny nvidia geforce, 8gb xlr8, gaming revel epic, rgb, dual fan - vcg3060t8ldfxppb1</t>
-        </is>
-      </c>
-      <c r="B64" t="n">
-        <v>3205.99</v>
-      </c>
-      <c r="C64" t="inlineStr">
-        <is>
-          <t>https://www.buscape.com.br/lead?oid=902491304&amp;channel=86&amp;index=9&amp;searchterm=rtx%203060</t>
-        </is>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="inlineStr">
-        <is>
-          <t>placa de vídeo rtx 3060 ti dual o8g v2 asus nvidia geforce, 8gb gddr6, rgb, dlss, lhr, ray tracing - dual-rtx3060ti-o8g-v2</t>
-        </is>
-      </c>
-      <c r="B65" t="n">
-        <v>3299.99</v>
-      </c>
-      <c r="C65" t="inlineStr">
-        <is>
-          <t>https://www.buscape.com.br/lead?oid=739872414&amp;channel=86&amp;index=10&amp;searchterm=rtx%203060</t>
-        </is>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="inlineStr">
-        <is>
-          <t>placa de vídeo rtx 3060 asus dual o12g v2 nvidia geforce, 12gb gddr6, lhr, dlss, ray tracing - dual-rtx3060-o12g-v2</t>
-        </is>
-      </c>
-      <c r="B66" t="n">
-        <v>2599.99</v>
-      </c>
-      <c r="C66" t="inlineStr">
-        <is>
-          <t>https://www.buscape.com.br/lead?oid=699424736&amp;channel=86&amp;index=12&amp;searchterm=rtx%203060</t>
-        </is>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="inlineStr">
-        <is>
-          <t>gigabyte placa de vídeo geforce rtx 3060 gaming oc 12g (rev2.0), 3x ventiladores windforce 12gb 192-bit gddr6, gv-n3060gaming oc-12gd rev2.0</t>
-        </is>
-      </c>
-      <c r="B67" t="n">
-        <v>4499</v>
-      </c>
-      <c r="C67" t="inlineStr">
-        <is>
-          <t>https://www.buscape.com.br/lead?oid=546338771&amp;channel=86&amp;index=13&amp;searchterm=rtx%203060</t>
-        </is>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="inlineStr">
-        <is>
-          <t>placa de vídeo rtx 3060 o12g v2 gaming asus tuf, 12gb gddr6, rgb, lhr, dlss, ray tracing - tuf-rtx3060-o12g-v2-gaming</t>
-        </is>
-      </c>
-      <c r="B68" t="n">
-        <v>3399.99</v>
-      </c>
-      <c r="C68" t="inlineStr">
-        <is>
-          <t>https://www.buscape.com.br/lead?oid=834707329&amp;channel=86&amp;index=14&amp;searchterm=rtx%203060</t>
-        </is>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="inlineStr">
-        <is>
-          <t>placa de vídeo asus gaming - geforce dual rtx 3060, 12gb gddr6, rgb, lhr, ray tracing, dlss</t>
-        </is>
-      </c>
-      <c r="B69" t="n">
-        <v>3058.81</v>
-      </c>
-      <c r="C69" t="inlineStr">
         <is>
           <t>https://www.buscape.com.br/lead?oid=419400087&amp;channel=86&amp;index=15&amp;searchterm=rtx%203060</t>
         </is>

</xml_diff>